<commit_message>
Commit sửa tên Tran Cao Len thành Tran Tan Len @@
</commit_message>
<xml_diff>
--- a/report/Tasksheet.xlsx
+++ b/report/Tasksheet.xlsx
@@ -360,9 +360,6 @@
     <t>Pham Hong Sang</t>
   </si>
   <si>
-    <t>Tran Cao Len</t>
-  </si>
-  <si>
     <t>Ha Chi Danh</t>
   </si>
   <si>
@@ -409,6 +406,9 @@
   </si>
   <si>
     <t>Change Password</t>
+  </si>
+  <si>
+    <t>Tran Tan Len</t>
   </si>
 </sst>
 </file>
@@ -660,30 +660,30 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -989,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView tabSelected="1" topLeftCell="B94" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1003,7 +1003,7 @@
     <col min="7" max="7" width="6.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="96.75">
+    <row r="1" spans="1:9" ht="96">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1020,10 +1020,10 @@
         <v>26</v>
       </c>
       <c r="F1" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="17" t="s">
         <v>78</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>79</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>18</v>
@@ -1033,10 +1033,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75">
-      <c r="A2" s="33">
+      <c r="A2" s="40">
         <v>1</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="40" t="s">
         <v>30</v>
       </c>
       <c r="C2" s="14" t="s">
@@ -1052,8 +1052,8 @@
       <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:9" ht="15.75">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
       <c r="C3" s="4" t="s">
         <v>27</v>
       </c>
@@ -1067,8 +1067,8 @@
       <c r="I3" s="13"/>
     </row>
     <row r="4" spans="1:9" ht="15.75">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
@@ -1082,8 +1082,8 @@
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" ht="15.75">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="41"/>
       <c r="C5" s="4" t="s">
         <v>28</v>
       </c>
@@ -1097,8 +1097,8 @@
       <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:9" ht="15.75">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1112,8 +1112,8 @@
       <c r="I6" s="13"/>
     </row>
     <row r="7" spans="1:9" ht="15.75">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="4" t="s">
         <v>29</v>
       </c>
@@ -1127,10 +1127,10 @@
       <c r="I7" s="13"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A8" s="34">
+      <c r="A8" s="41">
         <v>2</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="38" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1146,8 +1146,8 @@
       <c r="I8" s="13"/>
     </row>
     <row r="9" spans="1:9" ht="15.75">
-      <c r="A9" s="34"/>
-      <c r="B9" s="36"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="4" t="s">
         <v>32</v>
       </c>
@@ -1161,8 +1161,8 @@
       <c r="I9" s="13"/>
     </row>
     <row r="10" spans="1:9" ht="15.75">
-      <c r="A10" s="34"/>
-      <c r="B10" s="36"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="39"/>
       <c r="C10" s="4" t="s">
         <v>33</v>
       </c>
@@ -1176,8 +1176,8 @@
       <c r="I10" s="13"/>
     </row>
     <row r="11" spans="1:9" ht="15.75">
-      <c r="A11" s="34"/>
-      <c r="B11" s="33"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="4" t="s">
         <v>8</v>
       </c>
@@ -1191,8 +1191,8 @@
       <c r="I11" s="13"/>
     </row>
     <row r="12" spans="1:9" ht="15.75">
-      <c r="A12" s="34"/>
-      <c r="B12" s="35" t="s">
+      <c r="A12" s="41"/>
+      <c r="B12" s="38" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -1206,10 +1206,10 @@
       <c r="I12" s="13"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A13" s="34">
+      <c r="A13" s="41">
         <v>3</v>
       </c>
-      <c r="B13" s="36"/>
+      <c r="B13" s="39"/>
       <c r="C13" s="31" t="s">
         <v>35</v>
       </c>
@@ -1221,8 +1221,8 @@
       <c r="I13" s="13"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A14" s="34"/>
-      <c r="B14" s="36"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="39"/>
       <c r="C14" s="30" t="s">
         <v>47</v>
       </c>
@@ -1235,8 +1235,8 @@
       <c r="I14" s="13"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A15" s="34"/>
-      <c r="B15" s="36"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="30" t="s">
         <v>75</v>
       </c>
@@ -1250,10 +1250,10 @@
       <c r="I15" s="13"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A16" s="34"/>
-      <c r="B16" s="36"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1265,8 +1265,8 @@
       <c r="I16" s="13"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A17" s="34"/>
-      <c r="B17" s="36"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="39"/>
       <c r="C17" s="30" t="s">
         <v>76</v>
       </c>
@@ -1278,8 +1278,8 @@
       <c r="I17" s="13"/>
     </row>
     <row r="18" spans="1:9" ht="15.75">
-      <c r="A18" s="34"/>
-      <c r="B18" s="36"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="39"/>
       <c r="C18" s="31" t="s">
         <v>36</v>
       </c>
@@ -1291,10 +1291,10 @@
       <c r="I18" s="13"/>
     </row>
     <row r="19" spans="1:9" ht="15.75">
-      <c r="A19" s="34"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="39"/>
       <c r="C19" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1306,10 +1306,10 @@
       <c r="I19" s="13"/>
     </row>
     <row r="20" spans="1:9" ht="15.75">
-      <c r="A20" s="34"/>
-      <c r="B20" s="36"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1321,10 +1321,10 @@
       <c r="I20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="15.75">
-      <c r="A21" s="34"/>
-      <c r="B21" s="36"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="39"/>
       <c r="C21" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -1336,8 +1336,8 @@
       <c r="I21" s="13"/>
     </row>
     <row r="22" spans="1:9" ht="15.75">
-      <c r="A22" s="34"/>
-      <c r="B22" s="36"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="39"/>
       <c r="C22" s="30" t="s">
         <v>76</v>
       </c>
@@ -1349,8 +1349,8 @@
       <c r="I22" s="13"/>
     </row>
     <row r="23" spans="1:9" ht="15.75">
-      <c r="A23" s="34"/>
-      <c r="B23" s="36"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="39"/>
       <c r="C23" s="31" t="s">
         <v>37</v>
       </c>
@@ -1362,8 +1362,8 @@
       <c r="I23" s="13"/>
     </row>
     <row r="24" spans="1:9" ht="15.75">
-      <c r="A24" s="34"/>
-      <c r="B24" s="36"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="39"/>
       <c r="C24" s="30" t="s">
         <v>59</v>
       </c>
@@ -1377,10 +1377,10 @@
       <c r="I24" s="13"/>
     </row>
     <row r="25" spans="1:9" ht="15.75">
-      <c r="A25" s="34"/>
-      <c r="B25" s="36"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="39"/>
       <c r="C25" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2" t="s">
@@ -1392,10 +1392,10 @@
       <c r="I25" s="13"/>
     </row>
     <row r="26" spans="1:9" ht="15.75">
-      <c r="A26" s="34"/>
-      <c r="B26" s="36"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="39"/>
       <c r="C26" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>6</v>
@@ -1407,8 +1407,8 @@
       <c r="I26" s="13"/>
     </row>
     <row r="27" spans="1:9" ht="15.75">
-      <c r="A27" s="34"/>
-      <c r="B27" s="36"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="39"/>
       <c r="C27" s="30" t="s">
         <v>61</v>
       </c>
@@ -1422,8 +1422,8 @@
       <c r="I27" s="13"/>
     </row>
     <row r="28" spans="1:9" ht="15.75">
-      <c r="A28" s="34"/>
-      <c r="B28" s="36"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="39"/>
       <c r="C28" s="30" t="s">
         <v>76</v>
       </c>
@@ -1435,8 +1435,8 @@
       <c r="I28" s="13"/>
     </row>
     <row r="29" spans="1:9" ht="15.75">
-      <c r="A29" s="34"/>
-      <c r="B29" s="36"/>
+      <c r="A29" s="41"/>
+      <c r="B29" s="39"/>
       <c r="C29" s="31" t="s">
         <v>38</v>
       </c>
@@ -1450,8 +1450,8 @@
       <c r="I29" s="13"/>
     </row>
     <row r="30" spans="1:9" ht="15.75">
-      <c r="A30" s="34"/>
-      <c r="B30" s="36"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="39"/>
       <c r="C30" s="31" t="s">
         <v>39</v>
       </c>
@@ -1463,10 +1463,10 @@
       <c r="I30" s="13"/>
     </row>
     <row r="31" spans="1:9" ht="15.75">
-      <c r="A31" s="34"/>
-      <c r="B31" s="36"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="39"/>
       <c r="C31" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>6</v>
@@ -1478,10 +1478,10 @@
       <c r="I31" s="13"/>
     </row>
     <row r="32" spans="1:9" ht="15.75">
-      <c r="A32" s="34"/>
-      <c r="B32" s="36"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="39"/>
       <c r="C32" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D32" s="20"/>
       <c r="E32" s="2" t="s">
@@ -1493,8 +1493,8 @@
       <c r="I32" s="13"/>
     </row>
     <row r="33" spans="1:9" ht="15.75">
-      <c r="A33" s="34"/>
-      <c r="B33" s="36"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="39"/>
       <c r="C33" s="7" t="s">
         <v>40</v>
       </c>
@@ -1508,8 +1508,8 @@
       <c r="I33" s="13"/>
     </row>
     <row r="34" spans="1:9" ht="15.75">
-      <c r="A34" s="34"/>
-      <c r="B34" s="36"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="39"/>
       <c r="C34" s="7" t="s">
         <v>41</v>
       </c>
@@ -1523,8 +1523,8 @@
       <c r="I34" s="13"/>
     </row>
     <row r="35" spans="1:9" ht="15.75">
-      <c r="A35" s="34"/>
-      <c r="B35" s="36"/>
+      <c r="A35" s="41"/>
+      <c r="B35" s="39"/>
       <c r="C35" s="7" t="s">
         <v>42</v>
       </c>
@@ -1538,10 +1538,10 @@
       <c r="I35" s="13"/>
     </row>
     <row r="36" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A36" s="35">
+      <c r="A36" s="38">
         <v>4</v>
       </c>
-      <c r="B36" s="35" t="s">
+      <c r="B36" s="38" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="8" t="s">
@@ -1555,8 +1555,8 @@
       <c r="I36" s="13"/>
     </row>
     <row r="37" spans="1:9" ht="15.75">
-      <c r="A37" s="36"/>
-      <c r="B37" s="36"/>
+      <c r="A37" s="39"/>
+      <c r="B37" s="39"/>
       <c r="C37" s="9" t="s">
         <v>44</v>
       </c>
@@ -1570,8 +1570,8 @@
       <c r="I37" s="13"/>
     </row>
     <row r="38" spans="1:9" ht="15.75">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
+      <c r="A38" s="39"/>
+      <c r="B38" s="39"/>
       <c r="C38" s="10" t="s">
         <v>10</v>
       </c>
@@ -1585,8 +1585,8 @@
       <c r="I38" s="13"/>
     </row>
     <row r="39" spans="1:9" ht="15.75">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
+      <c r="A39" s="39"/>
+      <c r="B39" s="39"/>
       <c r="C39" s="8" t="s">
         <v>11</v>
       </c>
@@ -1600,8 +1600,8 @@
       <c r="I39" s="13"/>
     </row>
     <row r="40" spans="1:9" ht="15.75">
-      <c r="A40" s="36"/>
-      <c r="B40" s="36"/>
+      <c r="A40" s="39"/>
+      <c r="B40" s="39"/>
       <c r="C40" s="9" t="s">
         <v>45</v>
       </c>
@@ -1613,8 +1613,8 @@
       <c r="I40" s="13"/>
     </row>
     <row r="41" spans="1:9" ht="15.75">
-      <c r="A41" s="36"/>
-      <c r="B41" s="36"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="39"/>
       <c r="C41" s="27" t="s">
         <v>46</v>
       </c>
@@ -1627,7 +1627,7 @@
     </row>
     <row r="42" spans="1:9" ht="15.75">
       <c r="A42" s="32"/>
-      <c r="B42" s="36"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="27"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -1638,7 +1638,7 @@
     </row>
     <row r="43" spans="1:9" ht="15.75">
       <c r="A43" s="22"/>
-      <c r="B43" s="36"/>
+      <c r="B43" s="39"/>
       <c r="C43" s="24" t="s">
         <v>12</v>
       </c>
@@ -1651,7 +1651,7 @@
     </row>
     <row r="44" spans="1:9" ht="15.75">
       <c r="A44" s="22"/>
-      <c r="B44" s="36"/>
+      <c r="B44" s="39"/>
       <c r="C44" s="23"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -1662,7 +1662,7 @@
     </row>
     <row r="45" spans="1:9" ht="15.75">
       <c r="A45" s="22"/>
-      <c r="B45" s="36"/>
+      <c r="B45" s="39"/>
       <c r="C45" s="25" t="s">
         <v>49</v>
       </c>
@@ -1675,7 +1675,7 @@
     </row>
     <row r="46" spans="1:9" ht="15.75">
       <c r="A46" s="22"/>
-      <c r="B46" s="36"/>
+      <c r="B46" s="39"/>
       <c r="C46" s="26" t="s">
         <v>50</v>
       </c>
@@ -1690,7 +1690,7 @@
     </row>
     <row r="47" spans="1:9" ht="15.75">
       <c r="A47" s="22"/>
-      <c r="B47" s="36"/>
+      <c r="B47" s="39"/>
       <c r="C47" s="26" t="s">
         <v>51</v>
       </c>
@@ -1705,7 +1705,7 @@
     </row>
     <row r="48" spans="1:9" ht="15.75">
       <c r="A48" s="22"/>
-      <c r="B48" s="36"/>
+      <c r="B48" s="39"/>
       <c r="C48" s="26" t="s">
         <v>52</v>
       </c>
@@ -1720,7 +1720,7 @@
     </row>
     <row r="49" spans="1:9" ht="15.75">
       <c r="A49" s="22"/>
-      <c r="B49" s="36"/>
+      <c r="B49" s="39"/>
       <c r="C49" s="25" t="s">
         <v>53</v>
       </c>
@@ -1733,7 +1733,7 @@
     </row>
     <row r="50" spans="1:9" ht="15.75">
       <c r="A50" s="22"/>
-      <c r="B50" s="36"/>
+      <c r="B50" s="39"/>
       <c r="C50" s="26" t="s">
         <v>54</v>
       </c>
@@ -1748,7 +1748,7 @@
     </row>
     <row r="51" spans="1:9" ht="15.75">
       <c r="A51" s="22"/>
-      <c r="B51" s="36"/>
+      <c r="B51" s="39"/>
       <c r="C51" s="25" t="s">
         <v>15</v>
       </c>
@@ -1761,7 +1761,7 @@
     </row>
     <row r="52" spans="1:9" ht="15.75">
       <c r="A52" s="22"/>
-      <c r="B52" s="36"/>
+      <c r="B52" s="39"/>
       <c r="C52" s="26" t="s">
         <v>55</v>
       </c>
@@ -1776,7 +1776,7 @@
     </row>
     <row r="53" spans="1:9" ht="15.75">
       <c r="A53" s="22"/>
-      <c r="B53" s="33"/>
+      <c r="B53" s="40"/>
       <c r="C53" s="29" t="s">
         <v>54</v>
       </c>
@@ -1788,10 +1788,10 @@
       <c r="I53" s="13"/>
     </row>
     <row r="54" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A54" s="37">
+      <c r="A54" s="35">
         <v>5</v>
       </c>
-      <c r="B54" s="35" t="s">
+      <c r="B54" s="38" t="s">
         <v>16</v>
       </c>
       <c r="C54" s="9" t="s">
@@ -1809,10 +1809,10 @@
       </c>
     </row>
     <row r="55" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A55" s="38"/>
-      <c r="B55" s="36"/>
+      <c r="A55" s="36"/>
+      <c r="B55" s="39"/>
       <c r="C55" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -1826,10 +1826,10 @@
       </c>
     </row>
     <row r="56" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A56" s="38"/>
-      <c r="B56" s="36"/>
+      <c r="A56" s="36"/>
+      <c r="B56" s="39"/>
       <c r="C56" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -1842,8 +1842,8 @@
       </c>
     </row>
     <row r="57" spans="1:9" ht="15.75">
-      <c r="A57" s="38"/>
-      <c r="B57" s="36"/>
+      <c r="A57" s="36"/>
+      <c r="B57" s="39"/>
       <c r="C57" s="9" t="s">
         <v>57</v>
       </c>
@@ -1859,8 +1859,8 @@
       </c>
     </row>
     <row r="58" spans="1:9" ht="15.75">
-      <c r="A58" s="38"/>
-      <c r="B58" s="36"/>
+      <c r="A58" s="36"/>
+      <c r="B58" s="39"/>
       <c r="C58" s="9" t="s">
         <v>47</v>
       </c>
@@ -1876,8 +1876,8 @@
       </c>
     </row>
     <row r="59" spans="1:9" ht="15.75">
-      <c r="A59" s="38"/>
-      <c r="B59" s="36"/>
+      <c r="A59" s="36"/>
+      <c r="B59" s="39"/>
       <c r="C59" s="9" t="s">
         <v>58</v>
       </c>
@@ -1893,10 +1893,10 @@
       </c>
     </row>
     <row r="60" spans="1:9" ht="15.75">
-      <c r="A60" s="38"/>
-      <c r="B60" s="36"/>
+      <c r="A60" s="36"/>
+      <c r="B60" s="39"/>
       <c r="C60" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -1910,10 +1910,10 @@
       </c>
     </row>
     <row r="61" spans="1:9" ht="15.75">
-      <c r="A61" s="38"/>
-      <c r="B61" s="36"/>
+      <c r="A61" s="36"/>
+      <c r="B61" s="39"/>
       <c r="C61" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2" t="s">
@@ -1927,8 +1927,8 @@
       </c>
     </row>
     <row r="62" spans="1:9" ht="15.75">
-      <c r="A62" s="38"/>
-      <c r="B62" s="36"/>
+      <c r="A62" s="36"/>
+      <c r="B62" s="39"/>
       <c r="C62" s="9" t="s">
         <v>55</v>
       </c>
@@ -1944,10 +1944,10 @@
       </c>
     </row>
     <row r="63" spans="1:9" ht="15.75">
-      <c r="A63" s="38"/>
-      <c r="B63" s="36"/>
+      <c r="A63" s="36"/>
+      <c r="B63" s="39"/>
       <c r="C63" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -1961,10 +1961,10 @@
       </c>
     </row>
     <row r="64" spans="1:9" ht="15.75">
-      <c r="A64" s="38"/>
-      <c r="B64" s="36"/>
+      <c r="A64" s="36"/>
+      <c r="B64" s="39"/>
       <c r="C64" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -1978,10 +1978,10 @@
       </c>
     </row>
     <row r="65" spans="1:9" ht="15.75">
-      <c r="A65" s="38"/>
-      <c r="B65" s="36"/>
+      <c r="A65" s="36"/>
+      <c r="B65" s="39"/>
       <c r="C65" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>6</v>
@@ -1995,8 +1995,8 @@
       </c>
     </row>
     <row r="66" spans="1:9" ht="15.75">
-      <c r="A66" s="38"/>
-      <c r="B66" s="36"/>
+      <c r="A66" s="36"/>
+      <c r="B66" s="39"/>
       <c r="C66" s="9" t="s">
         <v>59</v>
       </c>
@@ -2012,10 +2012,10 @@
       </c>
     </row>
     <row r="67" spans="1:9" ht="15.75">
-      <c r="A67" s="38"/>
-      <c r="B67" s="36"/>
+      <c r="A67" s="36"/>
+      <c r="B67" s="39"/>
       <c r="C67" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="2" t="s">
@@ -2029,12 +2029,12 @@
       </c>
     </row>
     <row r="68" spans="1:9" ht="15.75">
-      <c r="A68" s="38"/>
-      <c r="B68" s="36"/>
+      <c r="A68" s="36"/>
+      <c r="B68" s="39"/>
       <c r="C68" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D68" s="41"/>
+        <v>83</v>
+      </c>
+      <c r="D68" s="34"/>
       <c r="E68" s="20"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2" t="s">
@@ -2046,10 +2046,10 @@
       </c>
     </row>
     <row r="69" spans="1:9" ht="15.75">
-      <c r="A69" s="38"/>
-      <c r="B69" s="36"/>
+      <c r="A69" s="36"/>
+      <c r="B69" s="39"/>
       <c r="C69" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -2063,8 +2063,8 @@
       </c>
     </row>
     <row r="70" spans="1:9" ht="15.75">
-      <c r="A70" s="38"/>
-      <c r="B70" s="36"/>
+      <c r="A70" s="36"/>
+      <c r="B70" s="39"/>
       <c r="C70" s="9" t="s">
         <v>48</v>
       </c>
@@ -2080,13 +2080,13 @@
       </c>
     </row>
     <row r="71" spans="1:9" ht="15.75">
-      <c r="A71" s="38"/>
-      <c r="B71" s="36"/>
+      <c r="A71" s="36"/>
+      <c r="B71" s="39"/>
       <c r="C71" s="9" t="s">
         <v>60</v>
       </c>
       <c r="D71" s="2"/>
-      <c r="E71" s="41"/>
+      <c r="E71" s="34"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2" t="s">
         <v>6</v>
@@ -2097,8 +2097,8 @@
       </c>
     </row>
     <row r="72" spans="1:9" ht="15.75">
-      <c r="A72" s="38"/>
-      <c r="B72" s="36"/>
+      <c r="A72" s="36"/>
+      <c r="B72" s="39"/>
       <c r="C72" s="9" t="s">
         <v>61</v>
       </c>
@@ -2114,8 +2114,8 @@
       </c>
     </row>
     <row r="73" spans="1:9" ht="15.75">
-      <c r="A73" s="38"/>
-      <c r="B73" s="36"/>
+      <c r="A73" s="36"/>
+      <c r="B73" s="39"/>
       <c r="C73" s="9" t="s">
         <v>62</v>
       </c>
@@ -2132,7 +2132,7 @@
     </row>
     <row r="74" spans="1:9" ht="15.75">
       <c r="A74" s="21"/>
-      <c r="B74" s="36"/>
+      <c r="B74" s="39"/>
       <c r="C74" s="11" t="s">
         <v>63</v>
       </c>
@@ -2140,14 +2140,14 @@
         <v>6</v>
       </c>
       <c r="E74" s="2"/>
-      <c r="F74" s="41"/>
+      <c r="F74" s="34"/>
       <c r="G74" s="2"/>
       <c r="H74" s="13"/>
       <c r="I74" s="13"/>
     </row>
     <row r="75" spans="1:9" ht="15.75">
       <c r="A75" s="21"/>
-      <c r="B75" s="36"/>
+      <c r="B75" s="39"/>
       <c r="C75" s="29" t="s">
         <v>64</v>
       </c>
@@ -2162,7 +2162,7 @@
     </row>
     <row r="76" spans="1:9" ht="15.75">
       <c r="A76" s="21"/>
-      <c r="B76" s="36"/>
+      <c r="B76" s="39"/>
       <c r="C76" s="9" t="s">
         <v>65</v>
       </c>
@@ -2177,7 +2177,7 @@
     </row>
     <row r="77" spans="1:9" ht="15.75">
       <c r="A77" s="21"/>
-      <c r="B77" s="36"/>
+      <c r="B77" s="39"/>
       <c r="C77" s="9" t="s">
         <v>66</v>
       </c>
@@ -2190,7 +2190,7 @@
     </row>
     <row r="78" spans="1:9" ht="15.75">
       <c r="A78" s="21"/>
-      <c r="B78" s="36"/>
+      <c r="B78" s="39"/>
       <c r="C78" s="9" t="s">
         <v>67</v>
       </c>
@@ -2205,7 +2205,7 @@
     </row>
     <row r="79" spans="1:9" ht="15.75">
       <c r="A79" s="21"/>
-      <c r="B79" s="33"/>
+      <c r="B79" s="40"/>
       <c r="C79" s="29" t="s">
         <v>13</v>
       </c>
@@ -2217,10 +2217,10 @@
       <c r="I79" s="13"/>
     </row>
     <row r="80" spans="1:9" ht="15.75">
-      <c r="A80" s="37">
-        <v>6</v>
-      </c>
-      <c r="B80" s="35" t="s">
+      <c r="A80" s="35">
+        <v>6</v>
+      </c>
+      <c r="B80" s="38" t="s">
         <v>5</v>
       </c>
       <c r="C80" s="9" t="s">
@@ -2236,8 +2236,8 @@
       <c r="I80" s="13"/>
     </row>
     <row r="81" spans="1:9" ht="15.75">
-      <c r="A81" s="38"/>
-      <c r="B81" s="36"/>
+      <c r="A81" s="36"/>
+      <c r="B81" s="39"/>
       <c r="C81" s="9" t="s">
         <v>68</v>
       </c>
@@ -2251,8 +2251,8 @@
       <c r="I81" s="13"/>
     </row>
     <row r="82" spans="1:9" ht="15.75">
-      <c r="A82" s="38"/>
-      <c r="B82" s="36"/>
+      <c r="A82" s="36"/>
+      <c r="B82" s="39"/>
       <c r="C82" s="27" t="s">
         <v>70</v>
       </c>
@@ -2264,8 +2264,8 @@
       <c r="I82" s="13"/>
     </row>
     <row r="83" spans="1:9" ht="15.75">
-      <c r="A83" s="38"/>
-      <c r="B83" s="36"/>
+      <c r="A83" s="36"/>
+      <c r="B83" s="39"/>
       <c r="C83" s="28" t="s">
         <v>71</v>
       </c>
@@ -2279,8 +2279,8 @@
       <c r="I83" s="13"/>
     </row>
     <row r="84" spans="1:9" ht="15.75">
-      <c r="A84" s="38"/>
-      <c r="B84" s="36"/>
+      <c r="A84" s="36"/>
+      <c r="B84" s="39"/>
       <c r="C84" s="29" t="s">
         <v>72</v>
       </c>
@@ -2292,8 +2292,8 @@
       <c r="I84" s="13"/>
     </row>
     <row r="85" spans="1:9" ht="15.75">
-      <c r="A85" s="38"/>
-      <c r="B85" s="36"/>
+      <c r="A85" s="36"/>
+      <c r="B85" s="39"/>
       <c r="C85" s="28" t="s">
         <v>73</v>
       </c>
@@ -2307,10 +2307,10 @@
       <c r="I85" s="13"/>
     </row>
     <row r="86" spans="1:9" ht="15.75">
-      <c r="A86" s="38"/>
-      <c r="B86" s="36"/>
+      <c r="A86" s="36"/>
+      <c r="B86" s="39"/>
       <c r="C86" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
@@ -2322,8 +2322,8 @@
       <c r="I86" s="13"/>
     </row>
     <row r="87" spans="1:9" ht="15.75">
-      <c r="A87" s="38"/>
-      <c r="B87" s="36"/>
+      <c r="A87" s="36"/>
+      <c r="B87" s="39"/>
       <c r="C87" s="28" t="s">
         <v>74</v>
       </c>
@@ -2337,10 +2337,10 @@
       <c r="I87" s="13"/>
     </row>
     <row r="88" spans="1:9" ht="15.75">
-      <c r="A88" s="39"/>
-      <c r="B88" s="33"/>
+      <c r="A88" s="37"/>
+      <c r="B88" s="40"/>
       <c r="C88" s="4"/>
-      <c r="D88" s="41"/>
+      <c r="D88" s="34"/>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
@@ -2422,24 +2422,24 @@
       <c r="B96" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C96" s="40">
+      <c r="C96" s="33">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A13:A35"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B12:B35"/>
     <mergeCell ref="A80:A88"/>
     <mergeCell ref="B80:B88"/>
     <mergeCell ref="A54:A73"/>
     <mergeCell ref="A36:A41"/>
     <mergeCell ref="B36:B53"/>
     <mergeCell ref="B54:B79"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A13:A35"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B12:B35"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D33:D52 D2:E31 G2:G13 D54:D91 E69:E91 E32:E67 G15:G56 F2:F55 F57:G91">

</xml_diff>

<commit_message>
add to modifie LenTC -> LenTT
</commit_message>
<xml_diff>
--- a/report/Tasksheet.xlsx
+++ b/report/Tasksheet.xlsx
@@ -360,9 +360,6 @@
     <t>Pham Hong Sang</t>
   </si>
   <si>
-    <t>Tran Cao Len</t>
-  </si>
-  <si>
     <t>Ha Chi Danh</t>
   </si>
   <si>
@@ -415,6 +412,9 @@
   </si>
   <si>
     <t>Notify for User</t>
+  </si>
+  <si>
+    <t>Tran Tan Len</t>
   </si>
 </sst>
 </file>
@@ -670,6 +670,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -678,18 +690,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -995,8 +995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1026,10 +1026,10 @@
         <v>26</v>
       </c>
       <c r="F1" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="17" t="s">
         <v>78</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>79</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>18</v>
@@ -1039,10 +1039,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75">
-      <c r="A2" s="40">
+      <c r="A2" s="35">
         <v>1</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="35" t="s">
         <v>30</v>
       </c>
       <c r="C2" s="14" t="s">
@@ -1058,8 +1058,8 @@
       <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:9" ht="15.75">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
       <c r="C3" s="4" t="s">
         <v>27</v>
       </c>
@@ -1073,8 +1073,8 @@
       <c r="I3" s="13"/>
     </row>
     <row r="4" spans="1:9" ht="15.75">
-      <c r="A4" s="41"/>
-      <c r="B4" s="41"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
@@ -1088,8 +1088,8 @@
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" ht="15.75">
-      <c r="A5" s="41"/>
-      <c r="B5" s="41"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="4" t="s">
         <v>28</v>
       </c>
@@ -1103,8 +1103,8 @@
       <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:9" ht="15.75">
-      <c r="A6" s="41"/>
-      <c r="B6" s="41"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1118,8 +1118,8 @@
       <c r="I6" s="13"/>
     </row>
     <row r="7" spans="1:9" ht="15.75">
-      <c r="A7" s="41"/>
-      <c r="B7" s="41"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="4" t="s">
         <v>29</v>
       </c>
@@ -1133,10 +1133,10 @@
       <c r="I7" s="13"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A8" s="41">
+      <c r="A8" s="36">
         <v>2</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="37" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1152,8 +1152,8 @@
       <c r="I8" s="13"/>
     </row>
     <row r="9" spans="1:9" ht="15.75">
-      <c r="A9" s="41"/>
-      <c r="B9" s="39"/>
+      <c r="A9" s="36"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="4" t="s">
         <v>32</v>
       </c>
@@ -1167,8 +1167,8 @@
       <c r="I9" s="13"/>
     </row>
     <row r="10" spans="1:9" ht="15.75">
-      <c r="A10" s="41"/>
-      <c r="B10" s="39"/>
+      <c r="A10" s="36"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="4" t="s">
         <v>33</v>
       </c>
@@ -1182,8 +1182,8 @@
       <c r="I10" s="13"/>
     </row>
     <row r="11" spans="1:9" ht="15.75">
-      <c r="A11" s="41"/>
-      <c r="B11" s="40"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="4" t="s">
         <v>8</v>
       </c>
@@ -1197,8 +1197,8 @@
       <c r="I11" s="13"/>
     </row>
     <row r="12" spans="1:9" ht="15.75">
-      <c r="A12" s="41"/>
-      <c r="B12" s="38" t="s">
+      <c r="A12" s="36"/>
+      <c r="B12" s="37" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -1212,10 +1212,10 @@
       <c r="I12" s="13"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A13" s="41">
+      <c r="A13" s="36">
         <v>3</v>
       </c>
-      <c r="B13" s="39"/>
+      <c r="B13" s="38"/>
       <c r="C13" s="31" t="s">
         <v>35</v>
       </c>
@@ -1227,8 +1227,8 @@
       <c r="I13" s="13"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A14" s="41"/>
-      <c r="B14" s="39"/>
+      <c r="A14" s="36"/>
+      <c r="B14" s="38"/>
       <c r="C14" s="30" t="s">
         <v>47</v>
       </c>
@@ -1241,8 +1241,8 @@
       <c r="I14" s="13"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A15" s="41"/>
-      <c r="B15" s="39"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="38"/>
       <c r="C15" s="30" t="s">
         <v>75</v>
       </c>
@@ -1256,10 +1256,10 @@
       <c r="I15" s="13"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A16" s="41"/>
-      <c r="B16" s="39"/>
+      <c r="A16" s="36"/>
+      <c r="B16" s="38"/>
       <c r="C16" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1271,8 +1271,8 @@
       <c r="I16" s="13"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A17" s="41"/>
-      <c r="B17" s="39"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="38"/>
       <c r="C17" s="30" t="s">
         <v>76</v>
       </c>
@@ -1284,8 +1284,8 @@
       <c r="I17" s="13"/>
     </row>
     <row r="18" spans="1:9" ht="15.75">
-      <c r="A18" s="41"/>
-      <c r="B18" s="39"/>
+      <c r="A18" s="36"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="31" t="s">
         <v>36</v>
       </c>
@@ -1297,10 +1297,10 @@
       <c r="I18" s="13"/>
     </row>
     <row r="19" spans="1:9" ht="15.75">
-      <c r="A19" s="41"/>
-      <c r="B19" s="39"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="38"/>
       <c r="C19" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1312,10 +1312,10 @@
       <c r="I19" s="13"/>
     </row>
     <row r="20" spans="1:9" ht="15.75">
-      <c r="A20" s="41"/>
-      <c r="B20" s="39"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1327,10 +1327,10 @@
       <c r="I20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="15.75">
-      <c r="A21" s="41"/>
-      <c r="B21" s="39"/>
+      <c r="A21" s="36"/>
+      <c r="B21" s="38"/>
       <c r="C21" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -1342,8 +1342,8 @@
       <c r="I21" s="13"/>
     </row>
     <row r="22" spans="1:9" ht="15.75">
-      <c r="A22" s="41"/>
-      <c r="B22" s="39"/>
+      <c r="A22" s="36"/>
+      <c r="B22" s="38"/>
       <c r="C22" s="30" t="s">
         <v>76</v>
       </c>
@@ -1355,8 +1355,8 @@
       <c r="I22" s="13"/>
     </row>
     <row r="23" spans="1:9" ht="15.75">
-      <c r="A23" s="41"/>
-      <c r="B23" s="39"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="38"/>
       <c r="C23" s="31" t="s">
         <v>37</v>
       </c>
@@ -1368,8 +1368,8 @@
       <c r="I23" s="13"/>
     </row>
     <row r="24" spans="1:9" ht="15.75">
-      <c r="A24" s="41"/>
-      <c r="B24" s="39"/>
+      <c r="A24" s="36"/>
+      <c r="B24" s="38"/>
       <c r="C24" s="30" t="s">
         <v>59</v>
       </c>
@@ -1383,10 +1383,10 @@
       <c r="I24" s="13"/>
     </row>
     <row r="25" spans="1:9" ht="15.75">
-      <c r="A25" s="41"/>
-      <c r="B25" s="39"/>
+      <c r="A25" s="36"/>
+      <c r="B25" s="38"/>
       <c r="C25" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2" t="s">
@@ -1398,10 +1398,10 @@
       <c r="I25" s="13"/>
     </row>
     <row r="26" spans="1:9" ht="15.75">
-      <c r="A26" s="41"/>
-      <c r="B26" s="39"/>
+      <c r="A26" s="36"/>
+      <c r="B26" s="38"/>
       <c r="C26" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>6</v>
@@ -1413,8 +1413,8 @@
       <c r="I26" s="13"/>
     </row>
     <row r="27" spans="1:9" ht="15.75">
-      <c r="A27" s="41"/>
-      <c r="B27" s="39"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="38"/>
       <c r="C27" s="30" t="s">
         <v>61</v>
       </c>
@@ -1428,8 +1428,8 @@
       <c r="I27" s="13"/>
     </row>
     <row r="28" spans="1:9" ht="15.75">
-      <c r="A28" s="41"/>
-      <c r="B28" s="39"/>
+      <c r="A28" s="36"/>
+      <c r="B28" s="38"/>
       <c r="C28" s="30" t="s">
         <v>76</v>
       </c>
@@ -1441,8 +1441,8 @@
       <c r="I28" s="13"/>
     </row>
     <row r="29" spans="1:9" ht="15.75">
-      <c r="A29" s="41"/>
-      <c r="B29" s="39"/>
+      <c r="A29" s="36"/>
+      <c r="B29" s="38"/>
       <c r="C29" s="31" t="s">
         <v>38</v>
       </c>
@@ -1456,8 +1456,8 @@
       <c r="I29" s="13"/>
     </row>
     <row r="30" spans="1:9" ht="15.75">
-      <c r="A30" s="41"/>
-      <c r="B30" s="39"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="38"/>
       <c r="C30" s="31" t="s">
         <v>39</v>
       </c>
@@ -1469,10 +1469,10 @@
       <c r="I30" s="13"/>
     </row>
     <row r="31" spans="1:9" ht="15.75">
-      <c r="A31" s="41"/>
-      <c r="B31" s="39"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="38"/>
       <c r="C31" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>6</v>
@@ -1484,10 +1484,10 @@
       <c r="I31" s="13"/>
     </row>
     <row r="32" spans="1:9" ht="15.75">
-      <c r="A32" s="41"/>
-      <c r="B32" s="39"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="38"/>
       <c r="C32" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D32" s="20"/>
       <c r="E32" s="2" t="s">
@@ -1499,8 +1499,8 @@
       <c r="I32" s="13"/>
     </row>
     <row r="33" spans="1:9" ht="15.75">
-      <c r="A33" s="41"/>
-      <c r="B33" s="39"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="38"/>
       <c r="C33" s="7" t="s">
         <v>40</v>
       </c>
@@ -1514,8 +1514,8 @@
       <c r="I33" s="13"/>
     </row>
     <row r="34" spans="1:9" ht="15.75">
-      <c r="A34" s="41"/>
-      <c r="B34" s="39"/>
+      <c r="A34" s="36"/>
+      <c r="B34" s="38"/>
       <c r="C34" s="7" t="s">
         <v>41</v>
       </c>
@@ -1529,8 +1529,8 @@
       <c r="I34" s="13"/>
     </row>
     <row r="35" spans="1:9" ht="15.75">
-      <c r="A35" s="41"/>
-      <c r="B35" s="39"/>
+      <c r="A35" s="36"/>
+      <c r="B35" s="38"/>
       <c r="C35" s="7" t="s">
         <v>42</v>
       </c>
@@ -1544,10 +1544,10 @@
       <c r="I35" s="13"/>
     </row>
     <row r="36" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A36" s="38">
+      <c r="A36" s="37">
         <v>4</v>
       </c>
-      <c r="B36" s="38" t="s">
+      <c r="B36" s="37" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="8" t="s">
@@ -1561,8 +1561,8 @@
       <c r="I36" s="13"/>
     </row>
     <row r="37" spans="1:9" ht="15.75">
-      <c r="A37" s="39"/>
-      <c r="B37" s="39"/>
+      <c r="A37" s="38"/>
+      <c r="B37" s="38"/>
       <c r="C37" s="9" t="s">
         <v>44</v>
       </c>
@@ -1576,8 +1576,8 @@
       <c r="I37" s="13"/>
     </row>
     <row r="38" spans="1:9" ht="15.75">
-      <c r="A38" s="39"/>
-      <c r="B38" s="39"/>
+      <c r="A38" s="38"/>
+      <c r="B38" s="38"/>
       <c r="C38" s="10" t="s">
         <v>10</v>
       </c>
@@ -1591,8 +1591,8 @@
       <c r="I38" s="13"/>
     </row>
     <row r="39" spans="1:9" ht="15.75">
-      <c r="A39" s="39"/>
-      <c r="B39" s="39"/>
+      <c r="A39" s="38"/>
+      <c r="B39" s="38"/>
       <c r="C39" s="8" t="s">
         <v>11</v>
       </c>
@@ -1606,8 +1606,8 @@
       <c r="I39" s="13"/>
     </row>
     <row r="40" spans="1:9" ht="15.75">
-      <c r="A40" s="39"/>
-      <c r="B40" s="39"/>
+      <c r="A40" s="38"/>
+      <c r="B40" s="38"/>
       <c r="C40" s="9" t="s">
         <v>45</v>
       </c>
@@ -1619,8 +1619,8 @@
       <c r="I40" s="13"/>
     </row>
     <row r="41" spans="1:9" ht="15.75">
-      <c r="A41" s="39"/>
-      <c r="B41" s="39"/>
+      <c r="A41" s="38"/>
+      <c r="B41" s="38"/>
       <c r="C41" s="27" t="s">
         <v>46</v>
       </c>
@@ -1633,7 +1633,7 @@
     </row>
     <row r="42" spans="1:9" ht="15.75">
       <c r="A42" s="32"/>
-      <c r="B42" s="39"/>
+      <c r="B42" s="38"/>
       <c r="C42" s="27"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -1644,7 +1644,7 @@
     </row>
     <row r="43" spans="1:9" ht="15.75">
       <c r="A43" s="22"/>
-      <c r="B43" s="39"/>
+      <c r="B43" s="38"/>
       <c r="C43" s="24" t="s">
         <v>12</v>
       </c>
@@ -1657,7 +1657,7 @@
     </row>
     <row r="44" spans="1:9" ht="15.75">
       <c r="A44" s="22"/>
-      <c r="B44" s="39"/>
+      <c r="B44" s="38"/>
       <c r="C44" s="23"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -1668,7 +1668,7 @@
     </row>
     <row r="45" spans="1:9" ht="15.75">
       <c r="A45" s="22"/>
-      <c r="B45" s="39"/>
+      <c r="B45" s="38"/>
       <c r="C45" s="25" t="s">
         <v>49</v>
       </c>
@@ -1681,7 +1681,7 @@
     </row>
     <row r="46" spans="1:9" ht="15.75">
       <c r="A46" s="22"/>
-      <c r="B46" s="39"/>
+      <c r="B46" s="38"/>
       <c r="C46" s="26" t="s">
         <v>50</v>
       </c>
@@ -1696,7 +1696,7 @@
     </row>
     <row r="47" spans="1:9" ht="15.75">
       <c r="A47" s="22"/>
-      <c r="B47" s="39"/>
+      <c r="B47" s="38"/>
       <c r="C47" s="26" t="s">
         <v>51</v>
       </c>
@@ -1711,7 +1711,7 @@
     </row>
     <row r="48" spans="1:9" ht="15.75">
       <c r="A48" s="22"/>
-      <c r="B48" s="39"/>
+      <c r="B48" s="38"/>
       <c r="C48" s="26" t="s">
         <v>52</v>
       </c>
@@ -1726,7 +1726,7 @@
     </row>
     <row r="49" spans="1:9" ht="15.75">
       <c r="A49" s="22"/>
-      <c r="B49" s="39"/>
+      <c r="B49" s="38"/>
       <c r="C49" s="25" t="s">
         <v>53</v>
       </c>
@@ -1739,7 +1739,7 @@
     </row>
     <row r="50" spans="1:9" ht="15.75">
       <c r="A50" s="22"/>
-      <c r="B50" s="39"/>
+      <c r="B50" s="38"/>
       <c r="C50" s="26" t="s">
         <v>54</v>
       </c>
@@ -1754,7 +1754,7 @@
     </row>
     <row r="51" spans="1:9" ht="15.75">
       <c r="A51" s="22"/>
-      <c r="B51" s="39"/>
+      <c r="B51" s="38"/>
       <c r="C51" s="25" t="s">
         <v>15</v>
       </c>
@@ -1767,7 +1767,7 @@
     </row>
     <row r="52" spans="1:9" ht="15.75">
       <c r="A52" s="22"/>
-      <c r="B52" s="39"/>
+      <c r="B52" s="38"/>
       <c r="C52" s="26" t="s">
         <v>55</v>
       </c>
@@ -1782,7 +1782,7 @@
     </row>
     <row r="53" spans="1:9" ht="15.75">
       <c r="A53" s="22"/>
-      <c r="B53" s="40"/>
+      <c r="B53" s="35"/>
       <c r="C53" s="29" t="s">
         <v>54</v>
       </c>
@@ -1794,10 +1794,10 @@
       <c r="I53" s="13"/>
     </row>
     <row r="54" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A54" s="35">
+      <c r="A54" s="39">
         <v>5</v>
       </c>
-      <c r="B54" s="38" t="s">
+      <c r="B54" s="37" t="s">
         <v>16</v>
       </c>
       <c r="C54" s="9" t="s">
@@ -1815,10 +1815,10 @@
       </c>
     </row>
     <row r="55" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A55" s="36"/>
-      <c r="B55" s="39"/>
+      <c r="A55" s="40"/>
+      <c r="B55" s="38"/>
       <c r="C55" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -1832,10 +1832,10 @@
       </c>
     </row>
     <row r="56" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A56" s="36"/>
-      <c r="B56" s="39"/>
+      <c r="A56" s="40"/>
+      <c r="B56" s="38"/>
       <c r="C56" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -1849,8 +1849,8 @@
       </c>
     </row>
     <row r="57" spans="1:9" ht="15.75">
-      <c r="A57" s="36"/>
-      <c r="B57" s="39"/>
+      <c r="A57" s="40"/>
+      <c r="B57" s="38"/>
       <c r="C57" s="9" t="s">
         <v>57</v>
       </c>
@@ -1866,8 +1866,8 @@
       </c>
     </row>
     <row r="58" spans="1:9" ht="15.75">
-      <c r="A58" s="36"/>
-      <c r="B58" s="39"/>
+      <c r="A58" s="40"/>
+      <c r="B58" s="38"/>
       <c r="C58" s="9" t="s">
         <v>47</v>
       </c>
@@ -1883,8 +1883,8 @@
       </c>
     </row>
     <row r="59" spans="1:9" ht="15.75">
-      <c r="A59" s="36"/>
-      <c r="B59" s="39"/>
+      <c r="A59" s="40"/>
+      <c r="B59" s="38"/>
       <c r="C59" s="9" t="s">
         <v>58</v>
       </c>
@@ -1900,10 +1900,10 @@
       </c>
     </row>
     <row r="60" spans="1:9" ht="15.75">
-      <c r="A60" s="36"/>
-      <c r="B60" s="39"/>
+      <c r="A60" s="40"/>
+      <c r="B60" s="38"/>
       <c r="C60" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -1917,10 +1917,10 @@
       </c>
     </row>
     <row r="61" spans="1:9" ht="15.75">
-      <c r="A61" s="36"/>
-      <c r="B61" s="39"/>
+      <c r="A61" s="40"/>
+      <c r="B61" s="38"/>
       <c r="C61" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2" t="s">
@@ -1934,8 +1934,8 @@
       </c>
     </row>
     <row r="62" spans="1:9" ht="15.75">
-      <c r="A62" s="36"/>
-      <c r="B62" s="39"/>
+      <c r="A62" s="40"/>
+      <c r="B62" s="38"/>
       <c r="C62" s="9" t="s">
         <v>55</v>
       </c>
@@ -1951,10 +1951,10 @@
       </c>
     </row>
     <row r="63" spans="1:9" ht="15.75">
-      <c r="A63" s="36"/>
-      <c r="B63" s="39"/>
+      <c r="A63" s="40"/>
+      <c r="B63" s="38"/>
       <c r="C63" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -1968,10 +1968,10 @@
       </c>
     </row>
     <row r="64" spans="1:9" ht="15.75">
-      <c r="A64" s="36"/>
-      <c r="B64" s="39"/>
+      <c r="A64" s="40"/>
+      <c r="B64" s="38"/>
       <c r="C64" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -1985,10 +1985,10 @@
       </c>
     </row>
     <row r="65" spans="1:9" ht="15.75">
-      <c r="A65" s="36"/>
-      <c r="B65" s="39"/>
+      <c r="A65" s="40"/>
+      <c r="B65" s="38"/>
       <c r="C65" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>6</v>
@@ -2002,8 +2002,8 @@
       </c>
     </row>
     <row r="66" spans="1:9" ht="15.75">
-      <c r="A66" s="36"/>
-      <c r="B66" s="39"/>
+      <c r="A66" s="40"/>
+      <c r="B66" s="38"/>
       <c r="C66" s="9" t="s">
         <v>59</v>
       </c>
@@ -2019,10 +2019,10 @@
       </c>
     </row>
     <row r="67" spans="1:9" ht="15.75">
-      <c r="A67" s="36"/>
-      <c r="B67" s="39"/>
+      <c r="A67" s="40"/>
+      <c r="B67" s="38"/>
       <c r="C67" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="2" t="s">
@@ -2036,10 +2036,10 @@
       </c>
     </row>
     <row r="68" spans="1:9" ht="15.75">
-      <c r="A68" s="36"/>
-      <c r="B68" s="39"/>
+      <c r="A68" s="40"/>
+      <c r="B68" s="38"/>
       <c r="C68" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D68" s="34"/>
       <c r="E68" s="20"/>
@@ -2053,10 +2053,10 @@
       </c>
     </row>
     <row r="69" spans="1:9" ht="15.75">
-      <c r="A69" s="36"/>
-      <c r="B69" s="39"/>
+      <c r="A69" s="40"/>
+      <c r="B69" s="38"/>
       <c r="C69" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="20"/>
@@ -2070,10 +2070,10 @@
       </c>
     </row>
     <row r="70" spans="1:9" ht="15.75">
-      <c r="A70" s="36"/>
-      <c r="B70" s="39"/>
+      <c r="A70" s="40"/>
+      <c r="B70" s="38"/>
       <c r="C70" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="20"/>
@@ -2087,10 +2087,10 @@
       </c>
     </row>
     <row r="71" spans="1:9" ht="15.75">
-      <c r="A71" s="36"/>
-      <c r="B71" s="39"/>
+      <c r="A71" s="40"/>
+      <c r="B71" s="38"/>
       <c r="C71" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
@@ -2104,8 +2104,8 @@
       </c>
     </row>
     <row r="72" spans="1:9" ht="15.75">
-      <c r="A72" s="36"/>
-      <c r="B72" s="39"/>
+      <c r="A72" s="40"/>
+      <c r="B72" s="38"/>
       <c r="C72" s="9" t="s">
         <v>48</v>
       </c>
@@ -2121,8 +2121,8 @@
       </c>
     </row>
     <row r="73" spans="1:9" ht="15.75">
-      <c r="A73" s="36"/>
-      <c r="B73" s="39"/>
+      <c r="A73" s="40"/>
+      <c r="B73" s="38"/>
       <c r="C73" s="9" t="s">
         <v>60</v>
       </c>
@@ -2138,8 +2138,8 @@
       </c>
     </row>
     <row r="74" spans="1:9" ht="15.75">
-      <c r="A74" s="36"/>
-      <c r="B74" s="39"/>
+      <c r="A74" s="40"/>
+      <c r="B74" s="38"/>
       <c r="C74" s="9" t="s">
         <v>61</v>
       </c>
@@ -2155,8 +2155,8 @@
       </c>
     </row>
     <row r="75" spans="1:9" ht="15.75">
-      <c r="A75" s="36"/>
-      <c r="B75" s="39"/>
+      <c r="A75" s="40"/>
+      <c r="B75" s="38"/>
       <c r="C75" s="9" t="s">
         <v>62</v>
       </c>
@@ -2173,7 +2173,7 @@
     </row>
     <row r="76" spans="1:9" ht="15.75">
       <c r="A76" s="21"/>
-      <c r="B76" s="39"/>
+      <c r="B76" s="38"/>
       <c r="C76" s="11" t="s">
         <v>63</v>
       </c>
@@ -2188,7 +2188,7 @@
     </row>
     <row r="77" spans="1:9" ht="15.75">
       <c r="A77" s="21"/>
-      <c r="B77" s="39"/>
+      <c r="B77" s="38"/>
       <c r="C77" s="29" t="s">
         <v>64</v>
       </c>
@@ -2203,7 +2203,7 @@
     </row>
     <row r="78" spans="1:9" ht="15.75">
       <c r="A78" s="21"/>
-      <c r="B78" s="39"/>
+      <c r="B78" s="38"/>
       <c r="C78" s="9" t="s">
         <v>65</v>
       </c>
@@ -2218,7 +2218,7 @@
     </row>
     <row r="79" spans="1:9" ht="15.75">
       <c r="A79" s="21"/>
-      <c r="B79" s="39"/>
+      <c r="B79" s="38"/>
       <c r="C79" s="9" t="s">
         <v>66</v>
       </c>
@@ -2231,7 +2231,7 @@
     </row>
     <row r="80" spans="1:9" ht="15.75">
       <c r="A80" s="21"/>
-      <c r="B80" s="39"/>
+      <c r="B80" s="38"/>
       <c r="C80" s="9" t="s">
         <v>67</v>
       </c>
@@ -2246,7 +2246,7 @@
     </row>
     <row r="81" spans="1:9" ht="15.75">
       <c r="A81" s="21"/>
-      <c r="B81" s="40"/>
+      <c r="B81" s="35"/>
       <c r="C81" s="29" t="s">
         <v>13</v>
       </c>
@@ -2258,10 +2258,10 @@
       <c r="I81" s="13"/>
     </row>
     <row r="82" spans="1:9" ht="15.75">
-      <c r="A82" s="35">
-        <v>6</v>
-      </c>
-      <c r="B82" s="38" t="s">
+      <c r="A82" s="39">
+        <v>6</v>
+      </c>
+      <c r="B82" s="37" t="s">
         <v>5</v>
       </c>
       <c r="C82" s="9" t="s">
@@ -2277,8 +2277,8 @@
       <c r="I82" s="13"/>
     </row>
     <row r="83" spans="1:9" ht="15.75">
-      <c r="A83" s="36"/>
-      <c r="B83" s="39"/>
+      <c r="A83" s="40"/>
+      <c r="B83" s="38"/>
       <c r="C83" s="9" t="s">
         <v>68</v>
       </c>
@@ -2292,8 +2292,8 @@
       <c r="I83" s="13"/>
     </row>
     <row r="84" spans="1:9" ht="15.75">
-      <c r="A84" s="36"/>
-      <c r="B84" s="39"/>
+      <c r="A84" s="40"/>
+      <c r="B84" s="38"/>
       <c r="C84" s="27" t="s">
         <v>70</v>
       </c>
@@ -2305,8 +2305,8 @@
       <c r="I84" s="13"/>
     </row>
     <row r="85" spans="1:9" ht="15.75">
-      <c r="A85" s="36"/>
-      <c r="B85" s="39"/>
+      <c r="A85" s="40"/>
+      <c r="B85" s="38"/>
       <c r="C85" s="28" t="s">
         <v>71</v>
       </c>
@@ -2320,8 +2320,8 @@
       <c r="I85" s="13"/>
     </row>
     <row r="86" spans="1:9" ht="15.75">
-      <c r="A86" s="36"/>
-      <c r="B86" s="39"/>
+      <c r="A86" s="40"/>
+      <c r="B86" s="38"/>
       <c r="C86" s="29" t="s">
         <v>72</v>
       </c>
@@ -2333,8 +2333,8 @@
       <c r="I86" s="13"/>
     </row>
     <row r="87" spans="1:9" ht="15.75">
-      <c r="A87" s="36"/>
-      <c r="B87" s="39"/>
+      <c r="A87" s="40"/>
+      <c r="B87" s="38"/>
       <c r="C87" s="28" t="s">
         <v>73</v>
       </c>
@@ -2348,10 +2348,10 @@
       <c r="I87" s="13"/>
     </row>
     <row r="88" spans="1:9" ht="15.75">
-      <c r="A88" s="36"/>
-      <c r="B88" s="39"/>
+      <c r="A88" s="40"/>
+      <c r="B88" s="38"/>
       <c r="C88" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
@@ -2363,8 +2363,8 @@
       <c r="I88" s="13"/>
     </row>
     <row r="89" spans="1:9" ht="15.75">
-      <c r="A89" s="36"/>
-      <c r="B89" s="39"/>
+      <c r="A89" s="40"/>
+      <c r="B89" s="38"/>
       <c r="C89" s="28" t="s">
         <v>74</v>
       </c>
@@ -2378,8 +2378,8 @@
       <c r="I89" s="13"/>
     </row>
     <row r="90" spans="1:9" ht="15.75">
-      <c r="A90" s="37"/>
-      <c r="B90" s="40"/>
+      <c r="A90" s="41"/>
+      <c r="B90" s="35"/>
       <c r="C90" s="4"/>
       <c r="D90" s="34"/>
       <c r="E90" s="2"/>
@@ -2469,18 +2469,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A82:A90"/>
+    <mergeCell ref="B82:B90"/>
+    <mergeCell ref="A54:A75"/>
+    <mergeCell ref="A36:A41"/>
+    <mergeCell ref="B36:B53"/>
+    <mergeCell ref="B54:B81"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A13:A35"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="B12:B35"/>
-    <mergeCell ref="A82:A90"/>
-    <mergeCell ref="B82:B90"/>
-    <mergeCell ref="A54:A75"/>
-    <mergeCell ref="A36:A41"/>
-    <mergeCell ref="B36:B53"/>
-    <mergeCell ref="B54:B81"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D33:D52 D2:E31 G2:G13 D54:D93 E69:E93 E32:E67 G15:G56 F2:F55 F71:G93 F57:G68 G69:G70">

</xml_diff>